<commit_message>
50 out of 50 first syscalls start the analysis
</commit_message>
<xml_diff>
--- a/FOLDER_0_ENVIRONMENT_STUFF/SYSCALLS_LOCATION.xlsx
+++ b/FOLDER_0_ENVIRONMENT_STUFF/SYSCALLS_LOCATION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="217" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
   <si>
     <t>SYSCALL</t>
   </si>
@@ -53,9 +53,6 @@
     <t>SYSCALL_DEFINE3</t>
   </si>
   <si>
-    <t>type problem i8*</t>
-  </si>
-  <si>
     <t>chdir</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>fs/file.c</t>
   </si>
   <si>
-    <t>type problem struct *</t>
-  </si>
-  <si>
     <t>fchown</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>kernel/sys.c</t>
   </si>
   <si>
-    <t>asm + gep struct *</t>
-  </si>
-  <si>
     <t>getpid</t>
   </si>
   <si>
@@ -170,34 +161,16 @@
     <t>lstat</t>
   </si>
   <si>
-    <t>lstat64</t>
-  </si>
-  <si>
     <t>mmap</t>
   </si>
   <si>
-    <t>arch/sparc/kernel/sys_sparc_64.c</t>
+    <t>arch/x86/kernel/sys_x86_64.c</t>
   </si>
   <si>
     <t>SYSCALL_DEFINE6</t>
   </si>
   <si>
-    <t>arch/microblaze/kernel/sys_microblaze.c</t>
-  </si>
-  <si>
-    <t>mmap2</t>
-  </si>
-  <si>
-    <t>arch/s390/kernel/sys_s390.c</t>
-  </si>
-  <si>
-    <t>arch/x86/kernel/sys_x86_64.c</t>
-  </si>
-  <si>
-    <t>arch/tile/kernel/sys.c</t>
-  </si>
-  <si>
-    <t>mmap_pgoff</t>
+    <t>munmap</t>
   </si>
   <si>
     <t>mm/mmap.c</t>
@@ -206,9 +179,6 @@
     <t>mm/nommu.c</t>
   </si>
   <si>
-    <t>munmap</t>
-  </si>
-  <si>
     <t>nice</t>
   </si>
   <si>
@@ -230,15 +200,12 @@
     <t>fs/fhandle.c</t>
   </si>
   <si>
-    <t>pipe2</t>
+    <t>pipe</t>
   </si>
   <si>
     <t>fs/pipe.c</t>
   </si>
   <si>
-    <t>pipe</t>
-  </si>
-  <si>
     <t>readahead</t>
   </si>
   <si>
@@ -275,6 +242,9 @@
     <t>SYSCALL_DEFINE5</t>
   </si>
   <si>
+    <t>weird message</t>
+  </si>
+  <si>
     <t>select</t>
   </si>
   <si>
@@ -296,18 +266,9 @@
     <t>sendfile</t>
   </si>
   <si>
-    <t>sendfile64</t>
-  </si>
-  <si>
     <t>setgid</t>
   </si>
   <si>
-    <t>setgid16</t>
-  </si>
-  <si>
-    <t>kernel/uid16.c</t>
-  </si>
-  <si>
     <t>setrlimit</t>
   </si>
   <si>
@@ -320,9 +281,6 @@
     <t>setuid</t>
   </si>
   <si>
-    <t>setuid16</t>
-  </si>
-  <si>
     <t>shutdown</t>
   </si>
   <si>
@@ -341,13 +299,7 @@
     <t>fs/statfs.c</t>
   </si>
   <si>
-    <t>statfs64</t>
-  </si>
-  <si>
     <t>stat</t>
-  </si>
-  <si>
-    <t>stat64</t>
   </si>
   <si>
     <t>syslog</t>
@@ -413,6 +365,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -472,9 +425,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -494,10 +451,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -509,7 +466,8 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1683673469388"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6785714285714"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.515306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="2.53571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="2.53571428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -563,11 +521,11 @@
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0</v>
@@ -575,10 +533,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
@@ -595,10 +553,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
@@ -615,16 +573,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -635,16 +593,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -655,10 +613,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>8</v>
@@ -675,7 +633,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>10</v>
@@ -683,11 +641,11 @@
       <c r="C9" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>12</v>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0</v>
@@ -695,24 +653,30 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>11</v>
@@ -729,10 +693,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>11</v>
@@ -749,10 +713,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>11</v>
@@ -769,16 +733,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E14" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0</v>
@@ -789,13 +753,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -809,13 +773,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
@@ -829,16 +793,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
@@ -849,16 +813,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>0</v>
@@ -869,16 +833,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0</v>
@@ -889,7 +853,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>10</v>
@@ -897,8 +861,8 @@
       <c r="C20" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>12</v>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0</v>
@@ -909,13 +873,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -929,16 +893,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>0</v>
@@ -949,10 +913,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>11</v>
@@ -969,13 +933,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>1</v>
@@ -989,16 +953,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>0</v>
@@ -1009,57 +973,93 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>18</v>
+        <v>50</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C28" s="0" t="s">
-        <v>54</v>
+        <v>17</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,279 +1067,453 @@
         <v>56</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>54</v>
+      <c r="E32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>18</v>
+        <v>74</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>68</v>
+        <v>11</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>10</v>
@@ -1350,65 +1524,65 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>11</v>
@@ -1416,54 +1590,54 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>8</v>
@@ -1471,10 +1645,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>8</v>
@@ -1482,298 +1656,67 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B93" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>